<commit_message>
add EPAD seq to whitelist
</commit_message>
<xml_diff>
--- a/whitelist.xlsx
+++ b/whitelist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t xml:space="preserve">scan_type</t>
   </si>
@@ -58,21 +58,78 @@
     <t xml:space="preserve">B0_ALFA1</t>
   </si>
   <si>
+    <t xml:space="preserve">Ax DTI (64 direc) iso 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAG FSPGR 3D</t>
+  </si>
+  <si>
     <t xml:space="preserve">VM2DI CLEAR</t>
   </si>
   <si>
+    <t xml:space="preserve">CT 3.0 B30f</t>
+  </si>
+  <si>
     <t xml:space="preserve">QFLOW_CAROTID</t>
   </si>
   <si>
     <t xml:space="preserve">M2DI</t>
   </si>
   <si>
+    <t xml:space="preserve">RESTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAG FSPGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COR FSPGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AX FSPGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerebral Blood Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ax T2 FLAIR_FS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D ASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AX GRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXIAL T2 FRFSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">QFLOW_CSF</t>
   </si>
   <si>
+    <t xml:space="preserve">Fractional Aniso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotropic image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Axial T2-Star</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_SENSE2</t>
+  </si>
+  <si>
     <t xml:space="preserve">SV_PRESS_100_Myo_CHESS_Hipo</t>
   </si>
   <si>
+    <t xml:space="preserve">Axial T2W-TSE with Fat Sat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAIR_SAG</t>
+  </si>
+  <si>
     <t xml:space="preserve">WIP muti-b bajo max</t>
   </si>
   <si>
@@ -100,9 +157,42 @@
     <t xml:space="preserve">SV_PRESS_100_Myo_CHESS_Ang</t>
   </si>
   <si>
+    <t xml:space="preserve">MPRAGE_CORONAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">M0_ASL</t>
   </si>
   <si>
+    <t xml:space="preserve">EPAD-B0-RevPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-SE-fMRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-SE-fMRI-RevPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-ASL-M0-TR10s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-ASL-M0-TR10s-RevPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-SingleShell-DTI32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-rsfMRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-ASL-M0-TR2s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPAD-2D-pCASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_SAGITAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">VWIP sT1W_3D_TFE_HR_32 iso1.2 long AT SENSE</t>
   </si>
   <si>
@@ -133,6 +223,9 @@
     <t xml:space="preserve">RS_ALFA1</t>
   </si>
   <si>
+    <t xml:space="preserve">SOURCE - EPAD-2D-pCASL</t>
+  </si>
+  <si>
     <t xml:space="preserve">SE-fMRI-AP</t>
   </si>
   <si>
@@ -160,6 +253,9 @@
     <t xml:space="preserve">SV_PRESS_100_Myo_CHESS</t>
   </si>
   <si>
+    <t xml:space="preserve">Sag</t>
+  </si>
+  <si>
     <t xml:space="preserve">PET_FDG_4x5min_recon3</t>
   </si>
   <si>
@@ -170,6 +266,192 @@
   </si>
   <si>
     <t xml:space="preserve">PET_Flutemetamol_4x5min_recon3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSM_ALFA2-V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D-pCASL_ALFA2-V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTI-ECHO_ALFA2-V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DelRec - QSM_ALFA2-V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIP SOURCE - 3D-pCASL_T1RHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMPRAGE_CORONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFLAIR_AXIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_Sag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMPRAGE_Sag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMPRAGE_Cor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_COR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_AXIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_Sagittal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMPRAGE_Sagittal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sagittal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMPRAGE_SAGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rev_rs_fMRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sT1W_3D_TFE_MPRAGE_SENSE2 SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGUE_CORONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rs_fMRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXIAL_NRECON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAGITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGUE_AXIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASL-M0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-ASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0_PA Negative Blip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTI_high_iso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fMRI rest.st.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VWIP MPRAGE_Sagittal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rev_DTI_64DIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DTI_64DIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi_echo_modificada SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0_map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sT1W_3D_TFE_MPRAGE_SENSE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sT1W_3D_TFE_RECON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sT1W_3D_TFE_RECONSTRONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sT1W_3D_TFE_RECONMEDIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DelRec - FLAIR_SAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAIR_SAG_RECON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWIp MinIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cor 3mm gap 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAG 3mm gap 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AX FLAIR 3mm 0 gap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VWIP MPRAGE_SENSE2 SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAIR_FLAIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VWIP FLAIR_SAG SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sWIP pCASL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi_echo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIP B1_calibration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIP B0_map SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COR_NRECON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFLAIR_SAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFLAIR_TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MPRAGE_EPAD_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLAIR_EPAD_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2_EPAD_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFLAIR_SAG SENSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VFLAIR_AXIALSENSE</t>
   </si>
 </sst>
 </file>
@@ -288,10 +570,10 @@
   <dimension ref="A1:A171"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
   </cols>
@@ -376,7 +658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -396,7 +678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -406,7 +688,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -421,7 +703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -431,7 +713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -461,7 +743,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -491,7 +773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -501,7 +783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -511,7 +793,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -536,297 +818,485 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3"/>
+      <c r="A51" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3"/>
+      <c r="A52" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3"/>
+      <c r="A54" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3"/>
+      <c r="A55" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="3"/>
+      <c r="A56" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="3"/>
+      <c r="A57" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3"/>
+      <c r="A59" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3"/>
+      <c r="A60" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="3"/>
+      <c r="A61" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="3"/>
+      <c r="A62" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3"/>
+      <c r="A63" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="3"/>
+      <c r="A64" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="3"/>
+      <c r="A66" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="3"/>
+      <c r="A67" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="3"/>
+      <c r="A68" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="3"/>
+      <c r="A69" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="3"/>
+      <c r="A70" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3"/>
+      <c r="A71" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="3"/>
+      <c r="A72" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="3"/>
+      <c r="A73" s="3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="3"/>
+      <c r="A74" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3"/>
+      <c r="A77" s="3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3"/>
+      <c r="A78" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="3"/>
+      <c r="A79" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3"/>
+      <c r="A80" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="3"/>
+      <c r="A83" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="3"/>
+      <c r="A84" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3"/>
+      <c r="A85" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="3"/>
+      <c r="A86" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="3"/>
+      <c r="A87" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3"/>
+      <c r="A88" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="3"/>
+      <c r="A90" s="3" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3"/>
+      <c r="A91" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="3"/>
+      <c r="A92" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="3"/>
+      <c r="A93" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="3"/>
+      <c r="A94" s="3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="3"/>
+      <c r="A95" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="3"/>
+      <c r="A96" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="3"/>
+      <c r="A97" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="3"/>
+      <c r="A98" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="3"/>
+      <c r="A99" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3"/>
+      <c r="A100" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="3"/>
+      <c r="A101" s="3" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="3"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="3"/>
+      <c r="A102" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="3"/>
+      <c r="A104" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="3"/>
+      <c r="A105" s="3" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="3"/>
+      <c r="A106" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="3"/>
+      <c r="A107" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="3"/>
+      <c r="A108" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="3"/>
+      <c r="A109" s="3" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="3"/>
+      <c r="A110" s="3" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3"/>
+      <c r="A111" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="3"/>
+      <c r="A112" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3"/>
+      <c r="A113" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="3"/>
+      <c r="A114" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="3"/>
+      <c r="A115" s="3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="3"/>
+      <c r="A116" s="3" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="3"/>
+      <c r="A117" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3"/>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="3"/>
+      <c r="A118" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="3" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="3"/>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="3"/>
+      <c r="A120" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="3" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3"/>
+      <c r="A122" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="3"/>
+      <c r="A123" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="3"/>
+      <c r="A124" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="3"/>
+      <c r="A125" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="3"/>
+      <c r="A126" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="3"/>
+      <c r="A127" s="3" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="3"/>
+      <c r="A128" s="3" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="3"/>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="3"/>
+      <c r="A129" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="3"/>
+      <c r="A131" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="3"/>
+      <c r="A132" s="3" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="3"/>
+      <c r="A133" s="3" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="3"/>
+      <c r="A134" s="3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="3"/>
+      <c r="A135" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="3"/>
+      <c r="A136" s="3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="3"/>
+      <c r="A137" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="3"/>
+      <c r="A138" s="3" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="3"/>
+      <c r="A139" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="3"/>
+      <c r="A140" s="3" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="3"/>
+      <c r="A141" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="3"/>
+      <c r="A142" s="3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="3"/>
+      <c r="A143" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="3"/>
+      <c r="A144" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3"/>

</xml_diff>